<commit_message>
Completed access for extracting items, getting states and districts pending
</commit_message>
<xml_diff>
--- a/vajrang/RoboticEnterpriseFramework_Template/Data/Config.xlsx
+++ b/vajrang/RoboticEnterpriseFramework_Template/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/FrameworkTemplates/REFramework/VB/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pranavi\Documents\UiPath\RPA-Developer-in-30-Days\vajrang\RoboticEnterpriseFramework_Template\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08611476-B0E6-4DE6-A3E5-39E09340BD80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10248" yWindow="17508" windowWidth="21252" windowHeight="9444" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>Name</t>
   </si>
@@ -160,6 +160,12 @@
   </si>
   <si>
     <t>ProcessABCQueue</t>
+  </si>
+  <si>
+    <t>InputFilepath</t>
+  </si>
+  <si>
+    <t>Data\Input\input data states.xlsx</t>
   </si>
 </sst>
 </file>
@@ -538,7 +544,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -615,7 +621,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>